<commit_message>
fixed bug with predefined results
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.1.3.7.xlsx
+++ b/compat/tablesSchema.1.3.7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\tse_workspace\tse-data-reporting-tool\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DA328D-C958-4D55-9670-3723066BEDD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A4C29C-6FBF-44A4-A7E0-0EEE60D69035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="690" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="690" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -6535,11 +6535,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7405,7 +7405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="N35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>